<commit_message>
add locality constraint to legend
</commit_message>
<xml_diff>
--- a/Tables/Supp Table 8 - SubSetNetworks.xlsx
+++ b/Tables/Supp Table 8 - SubSetNetworks.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22550" windowHeight="7710"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22545" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>B</t>
   </si>
@@ -105,7 +105,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>HPO genes discovered with networks built from accessions subsets</t>
+      <t>Locality HPO genes discovered with networks built from accessions subsets</t>
     </r>
     <r>
       <rPr>
@@ -116,9 +116,12 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-The number of HPO genes discovered in full ZmPAN (503 accessions) and ZmRoot (46 accessions) networks was compared to networks built with a subset of accessions. Both ZmPAN and ZmRoot networks were re-built using a common set of 20 accessions. The ZmPAN network was re-built using 46 accessions consisting of the 20 common accessions and either 26 random or 26 CML biased accessions to simulate the number used in the full 46 accession ZmRoot network. Each network was analyzed for HPO genes in the 17 GWAS elements.
+The number of HPO genes discovered in full ZmPAN (503 accessions) and ZmRoot (46 accessions) networks was compared to networks built with a subset of accessions. Both ZmPAN and ZmRoot networks were re-built using a common set of 20 accessions. The ZmPAN network was re-built using 46 accessions consisting of the 20 common accessions and either 26 random or 26 CML biased accessions to simulate the number used in the full 46 accession ZmRoot network. Each network was analyzed for HPO genes in the 17 GWAS elements using locality.
 </t>
     </r>
+  </si>
+  <si>
+    <t>Total Ionome</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,35 +731,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.1796875" customWidth="1"/>
+    <col min="2" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -779,7 +782,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -802,7 +805,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -825,7 +828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -848,7 +851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -871,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -894,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
@@ -917,7 +920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
@@ -940,7 +943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
@@ -963,7 +966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
@@ -986,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
@@ -1032,7 +1035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
@@ -1055,7 +1058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>11</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>12</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>14</v>
       </c>
@@ -1147,7 +1150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>16</v>
       </c>
@@ -1191,6 +1194,35 @@
       </c>
       <c r="G20" s="18">
         <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <f>SUM(B4:B20)</f>
+        <v>267</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:G21" si="0">SUM(C4:C20)</f>
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>